<commit_message>
Engadida posibilidade de indicar nome do arquivo ao executar
</commit_message>
<xml_diff>
--- a/P3/cmake-build-debug/medidasBurbulla.xlsx
+++ b/P3/cmake-build-debug/medidasBurbulla.xlsx
@@ -1,25 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GrEI\1 Ano\2 Cuatrimestre\Programacion II\Exercicios\P3\cmake-build-debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GrEI\1 Ano\2 Cuatrimestre\Programacion II\Exercicios\P3\cmake-build-debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34E9A9B-4B2B-425A-A5BA-183E9C736CCD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tiemposBurbuja_pc" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+  <si>
+    <t>talla</t>
+  </si>
+  <si>
+    <t>segundos</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -500,53 +516,54 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,7 +581,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -626,7 +643,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1046,7 +1063,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1084,7 +1101,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1434567072"/>
@@ -1180,7 +1197,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1212,7 +1229,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1384523104"/>
@@ -1253,7 +1270,914 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Comparativa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Burbulla</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>310000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>320000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>330000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>340000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>350000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>360000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>370000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>380000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>410000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>420000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>430000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>440000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>470000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>480000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>490000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.42099999999999899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6719999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6870000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.4529999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.422000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.890999999999899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.5779999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.436999999999898</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.390999999999899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.594000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.89</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83.311999999999898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>108.875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>122.671999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>137.046999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>151.48500000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>164.65600000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>179.68799999999899</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>199.40600000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214.06200000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>232.96799999999899</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>253.18799999999899</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>274.26499999999902</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>294.875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>316.96899999999903</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>341.32799999999901</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>364.10899999999901</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>388.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>414.56299999999902</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>440.18700000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>467.51600000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>496.03100000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>524.15700000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>553.82799999999895</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>582.88999999999896</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>614.70299999999895</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>646.84400000000005</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>679.20299999999895</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>713.78099999999904</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>745.18799999999896</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>783.78099999999904</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>818.95299999999895</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>856.56200000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>917.90599999999904</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>977.64099999999905</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1015.235</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1091.5630000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E93-42A4-BF69-32F6155D116A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Selección</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]tiemposSeleccion_pc!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.53100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.766</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5619999999999905</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.8279999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.515999999999899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.453000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.936999999999898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.688000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.531000000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.063000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>105.265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120.015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>134.48500000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>154.218999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172.375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>192.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>219.328</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>244.140999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>257.51600000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>290.17200000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>320.06200000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>346.15600000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>372.68799999999902</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>395.608</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>424.20400000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>456.34399999999903</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>487.90600000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>509.09300000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>544.45299999999895</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>579.64200000000005</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>611.15700000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>645.60799999999904</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>680.43799999999896</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>727.40599999999904</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>769.14099999999905</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>793.95299999999895</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>886</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>931.40599999999904</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>977.63999999999896</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1088.1569999999899</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1139.9369999999899</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1192.0940000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1175.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1211.2819999999899</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1262.0619999999899</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1287.1089999999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5E93-42A4-BF69-32F6155D116A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1393072320"/>
+        <c:axId val="1395555632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1393072320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>talla</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1395555632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1395555632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>segundos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1393072320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1304,6 +2228,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
   <cs:axisTitle>
@@ -1800,6 +2764,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1845,8 +3325,313 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A7FC33-2926-48C5-93BE-99428500E397}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="tiemposSeleccion_pc"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="C2">
+            <v>0.53100000000000003</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="C3">
+            <v>2.14</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>4.766</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>8.5619999999999905</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>14.125</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>20.8279999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>27.515999999999899</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9">
+            <v>35.453000000000003</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10">
+            <v>45</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>53.936999999999898</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>66.688000000000002</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>80.531000000000006</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>91.063000000000002</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15">
+            <v>105.265</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16">
+            <v>120.015</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>134.48500000000001</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18">
+            <v>154.218999999999</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19">
+            <v>172.375</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20">
+            <v>192.25</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21">
+            <v>219.328</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22">
+            <v>244.140999999999</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23">
+            <v>257.51600000000002</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>290.17200000000003</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>320.06200000000001</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26">
+            <v>346.15600000000001</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>372.68799999999902</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>395.608</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>424.20400000000001</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30">
+            <v>456.34399999999903</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>487.90600000000001</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32">
+            <v>509.09300000000002</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>544.45299999999895</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>579.64200000000005</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>611.15700000000004</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>645.60799999999904</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>680.43799999999896</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>727.40599999999904</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39">
+            <v>769.14099999999905</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="C40">
+            <v>793.95299999999895</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="C41">
+            <v>824</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="C42">
+            <v>886</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="C43">
+            <v>931.40599999999904</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="C44">
+            <v>977.63999999999896</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="C45">
+            <v>1088.1569999999899</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="C46">
+            <v>1139.9369999999899</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="C47">
+            <v>1192.0940000000001</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="C48">
+            <v>1175.5</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="C49">
+            <v>1211.2819999999899</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="C50">
+            <v>1262.0619999999899</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="C51">
+            <v>1287.1089999999899</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2141,19 +3926,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection sqref="A1:B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>10000</v>
       </c>
@@ -2161,7 +3946,7 @@
         <v>0.42099999999999899</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20000</v>
       </c>
@@ -2169,7 +3954,7 @@
         <v>1.6719999999999899</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30000</v>
       </c>
@@ -2177,7 +3962,7 @@
         <v>3.782</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40000</v>
       </c>
@@ -2185,7 +3970,7 @@
         <v>6.6870000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>50000</v>
       </c>
@@ -2193,7 +3978,7 @@
         <v>10.4529999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60000</v>
       </c>
@@ -2201,7 +3986,7 @@
         <v>15.422000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>70000</v>
       </c>
@@ -2209,7 +3994,7 @@
         <v>20.890999999999899</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80000</v>
       </c>
@@ -2217,7 +4002,7 @@
         <v>27.5779999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>90000</v>
       </c>
@@ -2225,7 +4010,7 @@
         <v>34.436999999999898</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100000</v>
       </c>
@@ -2233,7 +4018,7 @@
         <v>42.390999999999899</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110000</v>
       </c>
@@ -2241,7 +4026,7 @@
         <v>51.594000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>120000</v>
       </c>
@@ -2249,7 +4034,7 @@
         <v>60.89</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>130000</v>
       </c>
@@ -2257,7 +4042,7 @@
         <v>71.75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>140000</v>
       </c>
@@ -2265,7 +4050,7 @@
         <v>83.311999999999898</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>150000</v>
       </c>
@@ -2273,7 +4058,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>160000</v>
       </c>
@@ -2281,7 +4066,7 @@
         <v>108.875</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>170000</v>
       </c>
@@ -2289,7 +4074,7 @@
         <v>122.671999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>180000</v>
       </c>
@@ -2297,7 +4082,7 @@
         <v>137.046999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>190000</v>
       </c>
@@ -2305,7 +4090,7 @@
         <v>151.48500000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>200000</v>
       </c>
@@ -2313,7 +4098,7 @@
         <v>164.65600000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>210000</v>
       </c>
@@ -2321,7 +4106,7 @@
         <v>179.68799999999899</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>220000</v>
       </c>
@@ -2329,7 +4114,7 @@
         <v>199.40600000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>230000</v>
       </c>
@@ -2337,7 +4122,7 @@
         <v>214.06200000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>240000</v>
       </c>
@@ -2345,7 +4130,7 @@
         <v>232.96799999999899</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>250000</v>
       </c>
@@ -2353,7 +4138,7 @@
         <v>253.18799999999899</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>260000</v>
       </c>
@@ -2361,7 +4146,7 @@
         <v>274.26499999999902</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>270000</v>
       </c>
@@ -2369,7 +4154,7 @@
         <v>294.875</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>280000</v>
       </c>
@@ -2377,7 +4162,7 @@
         <v>316.96899999999903</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>290000</v>
       </c>
@@ -2385,7 +4170,7 @@
         <v>341.32799999999901</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>300000</v>
       </c>
@@ -2393,7 +4178,7 @@
         <v>364.10899999999901</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>310000</v>
       </c>
@@ -2401,7 +4186,7 @@
         <v>388.25</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>320000</v>
       </c>
@@ -2409,7 +4194,7 @@
         <v>414.56299999999902</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>330000</v>
       </c>
@@ -2417,7 +4202,7 @@
         <v>440.18700000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>340000</v>
       </c>
@@ -2425,7 +4210,7 @@
         <v>467.51600000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>350000</v>
       </c>
@@ -2433,7 +4218,7 @@
         <v>496.03100000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>360000</v>
       </c>
@@ -2441,7 +4226,7 @@
         <v>524.15700000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>370000</v>
       </c>
@@ -2449,7 +4234,7 @@
         <v>553.82799999999895</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>380000</v>
       </c>
@@ -2457,7 +4242,7 @@
         <v>582.88999999999896</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>390000</v>
       </c>
@@ -2465,7 +4250,7 @@
         <v>614.70299999999895</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>400000</v>
       </c>
@@ -2473,7 +4258,7 @@
         <v>646.84400000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410000</v>
       </c>
@@ -2481,7 +4266,7 @@
         <v>679.20299999999895</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420000</v>
       </c>
@@ -2489,7 +4274,7 @@
         <v>713.78099999999904</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>430000</v>
       </c>
@@ -2497,7 +4282,7 @@
         <v>745.18799999999896</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>440000</v>
       </c>
@@ -2505,7 +4290,7 @@
         <v>783.78099999999904</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>450000</v>
       </c>
@@ -2513,7 +4298,7 @@
         <v>818.95299999999895</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>460000</v>
       </c>
@@ -2521,7 +4306,7 @@
         <v>856.56200000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>470000</v>
       </c>
@@ -2529,7 +4314,7 @@
         <v>917.90599999999904</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>480000</v>
       </c>
@@ -2537,7 +4322,7 @@
         <v>977.64099999999905</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>490000</v>
       </c>
@@ -2545,7 +4330,7 @@
         <v>1015.235</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>500000</v>
       </c>
@@ -2558,4 +4343,738 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6AFE92-A728-4F98-A797-F3D2B4538767}">
+  <dimension ref="A1:E51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.42099999999999899</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.6719999999999899</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>30000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.782</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4.766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>40000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.6870000000000003</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8.5619999999999905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10.4529999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>50000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>60000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>15.422000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>20.8279999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>70000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20.890999999999899</v>
+      </c>
+      <c r="D8" s="2">
+        <v>70000</v>
+      </c>
+      <c r="E8" s="1">
+        <v>27.515999999999899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>80000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>27.5779999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>80000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>35.453000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>90000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>34.436999999999898</v>
+      </c>
+      <c r="D10" s="2">
+        <v>90000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42.390999999999899</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>53.936999999999898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>110000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>51.594000000000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>110000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>66.688000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>120000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>60.89</v>
+      </c>
+      <c r="D13" s="2">
+        <v>120000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>80.531000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>130000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>71.75</v>
+      </c>
+      <c r="D14" s="2">
+        <v>130000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>91.063000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>140000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>83.311999999999898</v>
+      </c>
+      <c r="D15" s="2">
+        <v>140000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>105.265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>150000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>95</v>
+      </c>
+      <c r="D16" s="2">
+        <v>150000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>120.015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>160000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>108.875</v>
+      </c>
+      <c r="D17" s="2">
+        <v>160000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>134.48500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>170000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>122.671999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>170000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>154.218999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>180000</v>
+      </c>
+      <c r="B19" s="1">
+        <v>137.046999999999</v>
+      </c>
+      <c r="D19" s="2">
+        <v>180000</v>
+      </c>
+      <c r="E19" s="1">
+        <v>172.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>190000</v>
+      </c>
+      <c r="B20" s="1">
+        <v>151.48500000000001</v>
+      </c>
+      <c r="D20" s="2">
+        <v>190000</v>
+      </c>
+      <c r="E20" s="1">
+        <v>192.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>200000</v>
+      </c>
+      <c r="B21" s="1">
+        <v>164.65600000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>200000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>219.328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>210000</v>
+      </c>
+      <c r="B22" s="1">
+        <v>179.68799999999899</v>
+      </c>
+      <c r="D22" s="2">
+        <v>210000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>244.140999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>220000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>199.40600000000001</v>
+      </c>
+      <c r="D23" s="2">
+        <v>220000</v>
+      </c>
+      <c r="E23" s="1">
+        <v>257.51600000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>230000</v>
+      </c>
+      <c r="B24" s="1">
+        <v>214.06200000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>230000</v>
+      </c>
+      <c r="E24" s="1">
+        <v>290.17200000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>240000</v>
+      </c>
+      <c r="B25" s="1">
+        <v>232.96799999999899</v>
+      </c>
+      <c r="D25" s="2">
+        <v>240000</v>
+      </c>
+      <c r="E25" s="1">
+        <v>320.06200000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>250000</v>
+      </c>
+      <c r="B26" s="1">
+        <v>253.18799999999899</v>
+      </c>
+      <c r="D26" s="2">
+        <v>250000</v>
+      </c>
+      <c r="E26" s="1">
+        <v>346.15600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>260000</v>
+      </c>
+      <c r="B27" s="1">
+        <v>274.26499999999902</v>
+      </c>
+      <c r="D27" s="2">
+        <v>260000</v>
+      </c>
+      <c r="E27" s="1">
+        <v>372.68799999999902</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>270000</v>
+      </c>
+      <c r="B28" s="1">
+        <v>294.875</v>
+      </c>
+      <c r="D28" s="2">
+        <v>270000</v>
+      </c>
+      <c r="E28" s="1">
+        <v>395.608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>280000</v>
+      </c>
+      <c r="B29" s="1">
+        <v>316.96899999999903</v>
+      </c>
+      <c r="D29" s="2">
+        <v>280000</v>
+      </c>
+      <c r="E29" s="1">
+        <v>424.20400000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>290000</v>
+      </c>
+      <c r="B30" s="1">
+        <v>341.32799999999901</v>
+      </c>
+      <c r="D30" s="2">
+        <v>290000</v>
+      </c>
+      <c r="E30" s="1">
+        <v>456.34399999999903</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>300000</v>
+      </c>
+      <c r="B31" s="1">
+        <v>364.10899999999901</v>
+      </c>
+      <c r="D31" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E31" s="1">
+        <v>487.90600000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>310000</v>
+      </c>
+      <c r="B32" s="1">
+        <v>388.25</v>
+      </c>
+      <c r="D32" s="2">
+        <v>310000</v>
+      </c>
+      <c r="E32" s="1">
+        <v>509.09300000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>320000</v>
+      </c>
+      <c r="B33" s="1">
+        <v>414.56299999999902</v>
+      </c>
+      <c r="D33" s="2">
+        <v>320000</v>
+      </c>
+      <c r="E33" s="1">
+        <v>544.45299999999895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>330000</v>
+      </c>
+      <c r="B34" s="1">
+        <v>440.18700000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>330000</v>
+      </c>
+      <c r="E34" s="1">
+        <v>579.64200000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>340000</v>
+      </c>
+      <c r="B35" s="1">
+        <v>467.51600000000002</v>
+      </c>
+      <c r="D35" s="2">
+        <v>340000</v>
+      </c>
+      <c r="E35" s="1">
+        <v>611.15700000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>350000</v>
+      </c>
+      <c r="B36" s="1">
+        <v>496.03100000000001</v>
+      </c>
+      <c r="D36" s="2">
+        <v>350000</v>
+      </c>
+      <c r="E36" s="1">
+        <v>645.60799999999904</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>360000</v>
+      </c>
+      <c r="B37" s="1">
+        <v>524.15700000000004</v>
+      </c>
+      <c r="D37" s="2">
+        <v>360000</v>
+      </c>
+      <c r="E37" s="1">
+        <v>680.43799999999896</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>370000</v>
+      </c>
+      <c r="B38" s="1">
+        <v>553.82799999999895</v>
+      </c>
+      <c r="D38" s="2">
+        <v>370000</v>
+      </c>
+      <c r="E38" s="1">
+        <v>727.40599999999904</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>380000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>582.88999999999896</v>
+      </c>
+      <c r="D39" s="2">
+        <v>380000</v>
+      </c>
+      <c r="E39" s="1">
+        <v>769.14099999999905</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>390000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>614.70299999999895</v>
+      </c>
+      <c r="D40" s="2">
+        <v>390000</v>
+      </c>
+      <c r="E40" s="1">
+        <v>793.95299999999895</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>400000</v>
+      </c>
+      <c r="B41" s="1">
+        <v>646.84400000000005</v>
+      </c>
+      <c r="D41" s="2">
+        <v>400000</v>
+      </c>
+      <c r="E41" s="1">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>410000</v>
+      </c>
+      <c r="B42" s="1">
+        <v>679.20299999999895</v>
+      </c>
+      <c r="D42" s="2">
+        <v>410000</v>
+      </c>
+      <c r="E42" s="1">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>420000</v>
+      </c>
+      <c r="B43" s="1">
+        <v>713.78099999999904</v>
+      </c>
+      <c r="D43" s="2">
+        <v>420000</v>
+      </c>
+      <c r="E43" s="1">
+        <v>931.40599999999904</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>430000</v>
+      </c>
+      <c r="B44" s="1">
+        <v>745.18799999999896</v>
+      </c>
+      <c r="D44" s="2">
+        <v>430000</v>
+      </c>
+      <c r="E44" s="1">
+        <v>977.63999999999896</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>440000</v>
+      </c>
+      <c r="B45" s="1">
+        <v>783.78099999999904</v>
+      </c>
+      <c r="D45" s="2">
+        <v>440000</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1088.1569999999899</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>450000</v>
+      </c>
+      <c r="B46" s="1">
+        <v>818.95299999999895</v>
+      </c>
+      <c r="D46" s="2">
+        <v>450000</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1139.9369999999899</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>460000</v>
+      </c>
+      <c r="B47" s="1">
+        <v>856.56200000000001</v>
+      </c>
+      <c r="D47" s="2">
+        <v>460000</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1192.0940000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>470000</v>
+      </c>
+      <c r="B48" s="1">
+        <v>917.90599999999904</v>
+      </c>
+      <c r="D48" s="2">
+        <v>470000</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1175.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>480000</v>
+      </c>
+      <c r="B49" s="1">
+        <v>977.64099999999905</v>
+      </c>
+      <c r="D49" s="2">
+        <v>480000</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1211.2819999999899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>490000</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1015.235</v>
+      </c>
+      <c r="D50" s="2">
+        <v>490000</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1262.0619999999899</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>500000</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1091.5630000000001</v>
+      </c>
+      <c r="D51" s="2">
+        <v>500000</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1287.1089999999899</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>